<commit_message>
Merge files... I think (hope)?
</commit_message>
<xml_diff>
--- a/xls/inheritance.xlsx
+++ b/xls/inheritance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin Neighly\Dropbox\School\Grad\Dissertation\excel docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin Neighly\Dropbox\School\Grad\Dissertation\git\tableau\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="138">
   <si>
     <t>cm</t>
   </si>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t>Agnes, r. Richard Smith, had her lands seized in 1380 when it was discovered that she had married without license; No record of how much she paid to inherit</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
   <si>
     <t>Found in Account Roll (LL.10761)</t>
@@ -797,14 +794,15 @@
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N66" sqref="N66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -921,10 +919,7 @@
         <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="M3" t="s">
         <v>94</v>
@@ -1091,10 +1086,7 @@
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="M7" t="s">
         <v>94</v>
@@ -1480,9 +1472,6 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16" t="s">
-        <v>128</v>
-      </c>
       <c r="M16" t="s">
         <v>94</v>
       </c>
@@ -1521,9 +1510,6 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" t="s">
-        <v>128</v>
-      </c>
       <c r="M17" t="s">
         <v>94</v>
       </c>
@@ -2278,7 +2264,7 @@
         <v>94</v>
       </c>
       <c r="N35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -2814,10 +2800,7 @@
         <v>16</v>
       </c>
       <c r="J48" t="s">
-        <v>64</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="M48" t="s">
         <v>94</v>
@@ -2981,10 +2964,7 @@
         <v>16</v>
       </c>
       <c r="J52" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="M52" t="s">
         <v>94</v>
@@ -3180,10 +3160,7 @@
         <v>9</v>
       </c>
       <c r="J57" t="s">
-        <v>64</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="M57" t="s">
         <v>94</v>
@@ -3431,9 +3408,6 @@
       <c r="J63" t="s">
         <v>65</v>
       </c>
-      <c r="K63" t="s">
-        <v>85</v>
-      </c>
       <c r="M63" t="s">
         <v>94</v>
       </c>
@@ -3675,7 +3649,7 @@
         <v>94</v>
       </c>
       <c r="N69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -3692,7 +3666,7 @@
         <v>59</v>
       </c>
       <c r="E70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F70" t="s">
         <v>65</v>
@@ -3713,7 +3687,7 @@
         <v>94</v>
       </c>
       <c r="N70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -3739,7 +3713,7 @@
         <v>80</v>
       </c>
       <c r="H71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I71" t="s">
         <v>6</v>
@@ -3751,7 +3725,7 @@
         <v>94</v>
       </c>
       <c r="N71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -3768,7 +3742,7 @@
         <v>59</v>
       </c>
       <c r="E72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F72" t="s">
         <v>65</v>
@@ -3789,7 +3763,7 @@
         <v>94</v>
       </c>
       <c r="N72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -3815,7 +3789,7 @@
         <v>248</v>
       </c>
       <c r="H73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I73" t="s">
         <v>6</v>
@@ -3830,7 +3804,7 @@
         <v>94</v>
       </c>
       <c r="N73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -3856,7 +3830,7 @@
         <v>160</v>
       </c>
       <c r="H74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I74" t="s">
         <v>9</v>
@@ -3871,7 +3845,7 @@
         <v>94</v>
       </c>
       <c r="N74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -3897,7 +3871,7 @@
         <v>3600</v>
       </c>
       <c r="H75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I75" t="s">
         <v>9</v>
@@ -3912,7 +3886,7 @@
         <v>94</v>
       </c>
       <c r="N75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>